<commit_message>
Update of the app3 shiny and addaptation of an excel file
</commit_message>
<xml_diff>
--- a/Data/Performance_sportive_et_nb_points.xlsx
+++ b/Data/Performance_sportive_et_nb_points.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,64 +24,64 @@
     <t>Fonction</t>
   </si>
   <si>
-    <t>Automobiliste</t>
-  </si>
-  <si>
     <t>min nb points</t>
   </si>
   <si>
-    <t>Canonnier</t>
-  </si>
-  <si>
-    <t>Canonnier lance-mine</t>
-  </si>
-  <si>
-    <t>Comptable de troupe</t>
-  </si>
-  <si>
-    <t>Cuisinier</t>
-  </si>
-  <si>
-    <t>Explorateur</t>
-  </si>
-  <si>
-    <t>Eclaireur</t>
-  </si>
-  <si>
-    <t>Fantassin</t>
-  </si>
-  <si>
     <t>Fusilier</t>
   </si>
   <si>
-    <t>Gren Isone-Char-Police militaire</t>
-  </si>
-  <si>
-    <t>Mécanicien</t>
-  </si>
-  <si>
-    <t>Ordonnance de bureau</t>
-  </si>
-  <si>
     <t>Pilot</t>
   </si>
   <si>
-    <t>Sanitaire</t>
-  </si>
-  <si>
-    <t>Soldat de renseignement</t>
-  </si>
-  <si>
-    <t>Soldat de transmission</t>
-  </si>
-  <si>
-    <t>Soldat d'artillerie</t>
-  </si>
-  <si>
-    <t>Soldat d'aviation</t>
-  </si>
-  <si>
-    <t>Spécialiste de montagne</t>
+    <t>Company Accountant</t>
+  </si>
+  <si>
+    <t>Troop Cook</t>
+  </si>
+  <si>
+    <t>Office Order</t>
+  </si>
+  <si>
+    <t>Cannoneer</t>
+  </si>
+  <si>
+    <t>Mechanic</t>
+  </si>
+  <si>
+    <t>Intelligence Soldier</t>
+  </si>
+  <si>
+    <t>Transmission Soldier</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Cannonballer</t>
+  </si>
+  <si>
+    <t>Infantryman</t>
+  </si>
+  <si>
+    <t>Sanitary</t>
+  </si>
+  <si>
+    <t>Artillery Soldier</t>
+  </si>
+  <si>
+    <t>Air Force Soldier</t>
+  </si>
+  <si>
+    <t>Explorer</t>
+  </si>
+  <si>
+    <t>Scout</t>
+  </si>
+  <si>
+    <t>Mountain Specialist</t>
+  </si>
+  <si>
+    <t>Grenadier - Isone, Char or Military Police</t>
   </si>
 </sst>
 </file>
@@ -135,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -143,17 +143,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +444,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -437,7 +455,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,161 +465,161 @@
     <col min="4" max="4" width="42.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
+    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>13</v>
+    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
+    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="B6" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>12</v>
+    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>16</v>
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="B8" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>17</v>
+    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>1</v>
+    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="B10" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>4</v>
+    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="B11" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>9</v>
+    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B12" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>15</v>
+    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B13" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>18</v>
+    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="B14" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>19</v>
+    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="B15" s="3">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>14</v>
+    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="B16" s="4">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>7</v>
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="B17" s="4">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>8</v>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="B18" s="4">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>20</v>
+    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>19</v>
       </c>
       <c r="B19" s="4">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>11</v>
+    <row r="20" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="B20" s="5">
         <v>90</v>
@@ -612,5 +630,6 @@
     <sortCondition ref="B2:B21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>